<commit_message>
chore : UserData 갑 수정
</commit_message>
<xml_diff>
--- a/Assets/Resources/UserData.xlsx
+++ b/Assets/Resources/UserData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\IdleSoul\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DF9802-74E9-4AD8-B274-ECE6F6EB97D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2789C161-EA4F-4AB3-BE99-E526A849349C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6FBF613A-6FA1-455C-A588-99C38EF2F98A}"/>
   </bookViews>
@@ -473,7 +473,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>